<commit_message>
Fixed bugs according to test case 1.0.9
</commit_message>
<xml_diff>
--- a/doc/ValidatorMessages.xlsx
+++ b/doc/ValidatorMessages.xlsx
@@ -121,18 +121,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -149,17 +143,65 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="7">
     <dxf>
       <fill>
-        <patternFill>
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -174,14 +216,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E10" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E10" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
   <autoFilter ref="A1:E10"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Message"/>
-    <tableColumn id="5" name="Priority" dataDxfId="0"/>
-    <tableColumn id="4" name="Table"/>
-    <tableColumn id="3" name="Colour"/>
-    <tableColumn id="2" name="Event"/>
+    <tableColumn id="1" name="Message" dataDxfId="6"/>
+    <tableColumn id="5" name="Priority" dataDxfId="5"/>
+    <tableColumn id="4" name="Table" dataDxfId="4"/>
+    <tableColumn id="3" name="Colour" dataDxfId="3"/>
+    <tableColumn id="2" name="Event" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -477,7 +519,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,51 +529,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -542,13 +584,13 @@
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -576,13 +618,13 @@
       <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -593,10 +635,10 @@
       <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -610,10 +652,10 @@
       <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -627,13 +669,13 @@
       <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -644,13 +686,13 @@
       <c r="B10" s="1">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>